<commit_message>
fix failed test cases
</commit_message>
<xml_diff>
--- a/documents/TestCases.xlsx
+++ b/documents/TestCases.xlsx
@@ -1011,7 +1011,6 @@
     <t>- User should be able to see the corresponding weather information in the content section for the selected option, including:
 + City name (should map with selected option).
 + Map section.
-+ Minute forecast section.
 + Hourly forecast section.
 + 8-day forecast section.</t>
   </si>
@@ -1235,16 +1234,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1260,11 +1258,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1828,10 +1827,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
@@ -1842,122 +1841,122 @@
       <c r="A3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="25">
         <v>44304.893055555556</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
@@ -2010,122 +2009,122 @@
       <c r="A18" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="25">
         <v>44304.893055555556</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="23"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
@@ -2178,122 +2177,122 @@
       <c r="A33" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="19">
+      <c r="B37" s="25">
         <v>44304.893055555556</v>
       </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="23"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="22"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
@@ -2350,122 +2349,122 @@
       <c r="A48" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B52" s="19">
+      <c r="B52" s="25">
         <v>44304.893055555556</v>
       </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="22"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="23"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="22"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="24" t="s">
+      <c r="B57" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B58" s="25" t="s">
+      <c r="B58" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
@@ -2491,7 +2490,7 @@
       <c r="B60" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C60" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -2506,7 +2505,7 @@
       <c r="B61" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C61" s="27"/>
+      <c r="C61" s="18"/>
       <c r="D61" s="2" t="s">
         <v>5</v>
       </c>
@@ -2514,31 +2513,16 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B24:E24"/>
@@ -2550,16 +2534,31 @@
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B58:E58"/>
   </mergeCells>
   <conditionalFormatting sqref="D15">
     <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
@@ -2653,7 +2652,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B21" sqref="B21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2673,56 +2672,56 @@
       <c r="A1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="25">
         <v>44304.893055555556</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -2739,56 +2738,56 @@
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -2822,7 +2821,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
@@ -2839,54 +2838,54 @@
       <c r="A16" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="25">
         <v>44304.90347222222</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
@@ -2903,56 +2902,56 @@
       <c r="A22" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
@@ -2990,56 +2989,56 @@
       <c r="A30" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="19">
+      <c r="B34" s="25">
         <v>44304.90347222222</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
@@ -3056,56 +3055,56 @@
       <c r="A36" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
@@ -3145,56 +3144,56 @@
       <c r="A44" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B48" s="19">
+      <c r="B48" s="25">
         <v>44304.90347222222</v>
       </c>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
@@ -3211,56 +3210,56 @@
       <c r="A50" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="24" t="s">
+      <c r="B53" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B54" s="25" t="s">
+      <c r="B54" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
@@ -3298,6 +3297,42 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B46:E46"/>
     <mergeCell ref="B52:E52"/>
     <mergeCell ref="B53:E53"/>
     <mergeCell ref="B54:E54"/>
@@ -3306,42 +3341,6 @@
     <mergeCell ref="B49:E49"/>
     <mergeCell ref="B50:E50"/>
     <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B10:E10"/>
   </mergeCells>
   <conditionalFormatting sqref="D13">
     <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">

</xml_diff>